<commit_message>
Modified json file again for Solis
</commit_message>
<xml_diff>
--- a/mapping_tools/modbus_devices_dbnpoller.xlsx
+++ b/mapping_tools/modbus_devices_dbnpoller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbaldwin/Work/2020/DS008-2020 (B4E-BUILDING)/rpiB4e/energy_poller/mapping_tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE99A7A7-26C4-E64E-A775-C1972F19CED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75334936-45A4-7343-93D7-D879A6F11DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17460" activeTab="8" xr2:uid="{5DD41FDB-13DA-47A3-8E54-3B553FBF34ED}"/>
   </bookViews>
@@ -14135,7 +14135,7 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14261,11 +14261,11 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" ref="B8:B52" si="0">IF(ISBLANK(A8),"",IF(AND($A8&gt;=0,($N8+$O8)&gt;$A8),"&lt;bad offset&gt;",$P8))</f>
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>80</v>
@@ -14309,7 +14309,7 @@
       </c>
       <c r="P8" s="10">
         <f>IF($A8&gt;=0,$A8,$N8+$O8)</f>
-        <v>3003</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -14334,7 +14334,7 @@
       </c>
       <c r="N9" s="10">
         <f>IF(ISNUMBER($N8),$P8,0)</f>
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="O9" s="10">
         <f t="shared" ref="O9:O52" ca="1" si="1">IF(ISNUMBER($H8),$H8,0)</f>

</xml_diff>